<commit_message>
#42: checking in challenge 2 content
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F532032D-E55B-B640-B4FB-2E522300C6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255128F8-87DC-9D41-AE90-0A9A9FC07388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105140" yWindow="-26000" windowWidth="41960" windowHeight="25220" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="105140" yWindow="-26000" windowWidth="41960" windowHeight="25220" activeTab="1" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Challenge 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -89,10 +90,6 @@
   </si>
   <si>
     <t>Security-related</t>
-  </si>
-  <si>
-    <t>Use the matrix below to determine the team's effectiveness in reaching the challenge objectives. The team should earn the
-required points in order to pass the challenge and move to the next. If the team does not reach the minimum point requirement, then encourage the team to spend more time in the necessary section(s) to improve their score.</t>
   </si>
   <si>
     <t>Possible points are based on the following scale:</t>
@@ -233,36 +230,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> in </t>
+      <t xml:space="preserve"> in each section to achieve success for the overall challenge.</t>
     </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>each section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to achieve success for the overall challenge.</t>
-    </r>
+  </si>
+  <si>
+    <t>Challenge 2: Operationalize automated deployments</t>
+  </si>
+  <si>
+    <t>Configure build/release pipelines in Azure</t>
+  </si>
+  <si>
+    <t>Configured build pipelines for all three projects</t>
+  </si>
+  <si>
+    <t>Configured release pipelines for all three projects</t>
+  </si>
+  <si>
+    <t>Configured and demonstrated approval gates for the production environment</t>
+  </si>
+  <si>
+    <t>Configured Bicep scripts to restrict which SKUs can be deployed</t>
+  </si>
+  <si>
+    <t>Determining a strategy for high-availability in deployments</t>
+  </si>
+  <si>
+    <t>Effictively explored various strategies for deployments</t>
+  </si>
+  <si>
+    <t>Successfully mapped a plan for maintaining uptime during deployments</t>
+  </si>
+  <si>
+    <t>Restricting Azure resource deployments</t>
+  </si>
+  <si>
+    <t>Configured a stage to show potential changes (e.g. "what-if") to production prior to release</t>
+  </si>
+  <si>
+    <t>Use the matrix below to determine the team's effectiveness in reaching the challenge objectives. The team should earn the required points in order to pass the challenge and move to the next. If the team does not reach the minimum point requirement, then encourage the team to spend more time in the necessary section(s) to improve their score.</t>
+  </si>
+  <si>
+    <t>Infrastructure deployments are non-destructive when applied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,14 +326,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -431,6 +438,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -453,6 +463,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984F1C9-37A0-284B-A0D6-38654FE3C443}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,78 +803,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="A4" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="31"/>
+      <c r="A6" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -869,13 +889,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -970,8 +990,8 @@
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="24" t="s">
-        <v>25</v>
+      <c r="F24" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -982,7 +1002,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="24"/>
+      <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -992,7 +1012,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="24"/>
+      <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -1002,7 +1022,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="24"/>
+      <c r="F27" s="25"/>
     </row>
     <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -1010,11 +1030,11 @@
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="25"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5">
@@ -1031,39 +1051,39 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="26" t="s">
-        <v>25</v>
+      <c r="F30" s="27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="26"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="26"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="26"/>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -1071,7 +1091,7 @@
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="26"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
@@ -1081,11 +1101,11 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="25"/>
+      <c r="F35" s="26"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5">
@@ -1102,7 +1122,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -1110,7 +1130,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -1119,7 +1139,7 @@
     <row r="39" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="17"/>
@@ -1128,7 +1148,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5">
@@ -1145,7 +1165,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -1153,7 +1173,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -1161,7 +1181,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -1169,7 +1189,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -1177,7 +1197,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -1185,7 +1205,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -1194,7 +1214,7 @@
     <row r="47" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="17"/>
@@ -1203,7 +1223,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5">
@@ -1219,17 +1239,17 @@
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="27"/>
+      <c r="A49" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="28"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -1238,7 +1258,7 @@
     <row r="51" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
       <c r="B51" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="17"/>
@@ -1256,4 +1276,250 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434FE90F-E318-8948-B8D8-94091A28442F}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5">
+        <v>16</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19">
+        <f>SUM(C23:C23)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="19">
+        <v>4</v>
+      </c>
+      <c r="E22" s="19">
+        <v>3</v>
+      </c>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5">
+        <f>SUM(C25:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>8</v>
+      </c>
+      <c r="E24" s="5">
+        <v>7</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#43: adding challenge 3
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255128F8-87DC-9D41-AE90-0A9A9FC07388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9ABFFE-BDB8-0B4F-9A45-89AD08EF7807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105140" yWindow="-26000" windowWidth="41960" windowHeight="25220" activeTab="1" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="2" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
     <sheet name="Challenge 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Challenge 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -271,6 +272,52 @@
   </si>
   <si>
     <t>Infrastructure deployments are non-destructive when applied</t>
+  </si>
+  <si>
+    <t>Challenge 3: Planning for failure</t>
+  </si>
+  <si>
+    <t>Alerting and monitoring</t>
+  </si>
+  <si>
+    <t>Provided a documented process for alerts and notifications</t>
+  </si>
+  <si>
+    <t>Identified events, criticality and business impact, responsibilies, and appropriate
+remediation steps</t>
+  </si>
+  <si>
+    <t>Alert(s) has been successfully sent for failed environment components</t>
+  </si>
+  <si>
+    <t>Log Analytics and Security Center has been enabled for all resources</t>
+  </si>
+  <si>
+    <t>Successfully configured logs to be retained for no less than 7 years</t>
+  </si>
+  <si>
+    <t>Azure Sentinel has been enabled</t>
+  </si>
+  <si>
+    <t>Demonstrated knowledge of using and querying Azure Sentinel</t>
+  </si>
+  <si>
+    <t>Business Continuity and Disaster Recovery</t>
+  </si>
+  <si>
+    <t>Provided a documented BCDR strategy and effectively communicated it</t>
+  </si>
+  <si>
+    <t>Composite SLA of environment is at least 99.99%</t>
+  </si>
+  <si>
+    <t>RTO and RPO meet or exceed Woodgrove Bank's SLA of 10 minutes and 1 hour, respectively</t>
+  </si>
+  <si>
+    <t>Successfully confiured a hot-hot, multi-region deployment</t>
+  </si>
+  <si>
+    <t>An initial, adequate RACI chart has been constructed and effectively communicated by the team</t>
   </si>
 </sst>
 </file>
@@ -405,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -437,6 +484,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -473,6 +523,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,44 +859,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -990,7 +1046,7 @@
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1002,7 +1058,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="25"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -1012,7 +1068,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="25"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -1022,7 +1078,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="25"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -1030,7 +1086,7 @@
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="26"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
@@ -1057,7 +1113,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1067,7 +1123,7 @@
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
@@ -1075,7 +1131,7 @@
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="27"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
@@ -1083,7 +1139,7 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="27"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -1091,7 +1147,7 @@
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="27"/>
+      <c r="F34" s="28"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
@@ -1101,7 +1157,7 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="26"/>
+      <c r="F35" s="27"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
@@ -1239,10 +1295,10 @@
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="28"/>
+      <c r="B49" s="29"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="21"/>
@@ -1282,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434FE90F-E318-8948-B8D8-94091A28442F}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1296,44 +1352,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1434,17 +1490,17 @@
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="35" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="16"/>
@@ -1477,7 +1533,7 @@
       <c r="C23" s="16"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="24"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
@@ -1512,7 +1568,274 @@
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="33"/>
+      <c r="F26" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4A77FD-B06A-CC44-B563-AB7667450FE9}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25:L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C23)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5">
+        <v>16</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="37"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="37"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19">
+        <f>SUM(C25:C25)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="19">
+        <v>4</v>
+      </c>
+      <c r="E24" s="19">
+        <v>3</v>
+      </c>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
#44: adding challenge 4
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9ABFFE-BDB8-0B4F-9A45-89AD08EF7807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7196CE-6E81-214F-91F3-64DEA2E43B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="2" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="3" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
     <sheet name="Challenge 2" sheetId="2" r:id="rId2"/>
     <sheet name="Challenge 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Challenge 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -318,6 +319,57 @@
   </si>
   <si>
     <t>An initial, adequate RACI chart has been constructed and effectively communicated by the team</t>
+  </si>
+  <si>
+    <t>Challenge 4: Visualizing operations</t>
+  </si>
+  <si>
+    <t>Operational dashboards</t>
+  </si>
+  <si>
+    <t>None: 0
+1 Board: 1
+2+ Boards: 2</t>
+  </si>
+  <si>
+    <t>How many dashboards did the team create that are:</t>
+  </si>
+  <si>
+    <t>Across these dashboards, how many panels did the team create that are:</t>
+  </si>
+  <si>
+    <t>None: 0
+1-2 Panelss: 1
+3-4 Panels: 2
+5-6 Panels: 3
+7+ Panels: 4</t>
+  </si>
+  <si>
+    <t>Cost-related</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Grafana can successfully connect to Log Analytics and Azure Monitor</t>
+  </si>
+  <si>
+    <t>Configured dashboards to auto-refresh every 10 seconds or less</t>
+  </si>
+  <si>
+    <t>Successfully demonstrated the dashboards cycling through</t>
+  </si>
+  <si>
+    <t>Successfully created appropriate permissions to differentiate between editors
+and viewers</t>
+  </si>
+  <si>
+    <t>Designed and effectively communicated their reasoning for why they organized 
+their dashboards the way they did</t>
+  </si>
+  <si>
+    <t>Presented a reasonable solution for storing and querying on-premises operational 
+data</t>
   </si>
 </sst>
 </file>
@@ -431,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -448,11 +500,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -528,6 +589,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,7 +915,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="F24" sqref="F24:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1339,7 +1408,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1584,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4A77FD-B06A-CC44-B563-AB7667450FE9}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25:L26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F16" s="21"/>
     </row>
@@ -1780,14 +1849,14 @@
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19">
-        <f>SUM(C25:C25)</f>
+        <f>SUM(C25:C29)</f>
         <v>0</v>
       </c>
       <c r="D24" s="19">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E24" s="19">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F24" s="20"/>
     </row>
@@ -1845,4 +1914,324 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC78BC-45CF-634D-A8AD-94D6AABF3885}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>54</v>
+      </c>
+      <c r="E16" s="5">
+        <v>44</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="26"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="26"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="27"/>
+    </row>
+    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="1:6" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="F23:F28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#45: adding challenge 5
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7196CE-6E81-214F-91F3-64DEA2E43B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C2FD62-65C7-C041-B953-1332AE290597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="3" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="4" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
     <sheet name="Challenge 2" sheetId="2" r:id="rId2"/>
     <sheet name="Challenge 3" sheetId="3" r:id="rId3"/>
     <sheet name="Challenge 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Challenge 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -370,6 +371,35 @@
   <si>
     <t>Presented a reasonable solution for storing and querying on-premises operational 
 data</t>
+  </si>
+  <si>
+    <t>Challenge 5: Improve the environment</t>
+  </si>
+  <si>
+    <t>Environment Improvements</t>
+  </si>
+  <si>
+    <t>How many improvements did the team implement that are:</t>
+  </si>
+  <si>
+    <t>None: 0
+1-2 Changes: 1
+2-5 Changes: 2
+5-9 Changes: 3
+10+ Changes: 4</t>
+  </si>
+  <si>
+    <t>Application Insights has been added to the application and Grafana has been 
+updated to report the collected metrics</t>
+  </si>
+  <si>
+    <t>Performance has been maintained or improved</t>
+  </si>
+  <si>
+    <t>Accurately and effectively communicated the ACHIEVE process</t>
+  </si>
+  <si>
+    <t>All changes have been implemented via Azure Bicep/ARM Templates</t>
   </si>
 </sst>
 </file>
@@ -924,7 +954,7 @@
     <col min="2" max="2" width="68.1640625" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1417,7 +1447,7 @@
     <col min="2" max="2" width="68.1640625" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1663,7 +1693,7 @@
     <col min="2" max="2" width="68.1640625" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1920,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC78BC-45CF-634D-A8AD-94D6AABF3885}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
@@ -1930,7 +1960,7 @@
     <col min="2" max="2" width="68.1640625" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2234,4 +2264,248 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400EB03E-F4EF-8741-A1B1-1EB5D473423F}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5">
+        <v>29</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="26"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="F24:F26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#43: adding additional resolution
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C2FD62-65C7-C041-B953-1332AE290597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFA744E-9357-1D45-9A9B-EB40D5B7B830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="4" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="2" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>All changes have been implemented via Azure Bicep/ARM Templates</t>
+  </si>
+  <si>
+    <t>Alerts have been configured to report approaching system thresholds</t>
+  </si>
+  <si>
+    <t>Alerts have been configured to report underutilized resources</t>
   </si>
 </sst>
 </file>
@@ -1681,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4A77FD-B06A-CC44-B563-AB7667450FE9}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1798,14 +1804,14 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5">
-        <f>SUM(C17:C23)</f>
+        <f>SUM(C17:C25)</f>
         <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E16" s="5">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F16" s="21"/>
     </row>
@@ -1834,107 +1840,123 @@
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="37"/>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="37"/>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="37"/>
     </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="39" t="s">
+    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="37"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19">
-        <f>SUM(C25:C29)</f>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19">
+        <f>SUM(C27:C31)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D26" s="19">
         <v>20</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E26" s="19">
         <v>16</v>
       </c>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15" t="s">
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="36" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="35" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="34"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2270,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400EB03E-F4EF-8741-A1B1-1EB5D473423F}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes #46: adding challenge 6
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10707"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFA744E-9357-1D45-9A9B-EB40D5B7B830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB96AA3-F961-6747-8F1A-B2B452E4146D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102960" yWindow="-27760" windowWidth="47480" windowHeight="27200" activeTab="2" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="103800" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Challenge 3" sheetId="3" r:id="rId3"/>
     <sheet name="Challenge 4" sheetId="4" r:id="rId4"/>
     <sheet name="Challenge 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Challenge 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -406,6 +407,46 @@
   </si>
   <si>
     <t>Alerts have been configured to report underutilized resources</t>
+  </si>
+  <si>
+    <t>Challenge 6: Leveraging PaaS services</t>
+  </si>
+  <si>
+    <t>Satisfactorily practiced the ACHIEVE process</t>
+  </si>
+  <si>
+    <t>Alerting is properly configured</t>
+  </si>
+  <si>
+    <t>Application continues to operate under failure</t>
+  </si>
+  <si>
+    <t>Azure App Services configured to autoscale up AND down</t>
+  </si>
+  <si>
+    <t>Azure App Service configurations are secure</t>
+  </si>
+  <si>
+    <t>Azure SQL has been configured for failover</t>
+  </si>
+  <si>
+    <t>Using Azure Key Vault for configuration and SQL Always Encrypted</t>
+  </si>
+  <si>
+    <t>Data connectivity and in transit is secure</t>
+  </si>
+  <si>
+    <t>Configured Azure Batch for processing background jobs</t>
+  </si>
+  <si>
+    <t>Reporting has been added/updated for PaaS services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None: 0
+1-2 Changes: 2
+3 Changes: 3
+4+ Changes: 4
+</t>
   </si>
 </sst>
 </file>
@@ -549,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -591,24 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -631,8 +654,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,44 +1011,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1151,7 +1198,7 @@
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1163,7 +1210,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -1173,7 +1220,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -1183,7 +1230,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="26"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -1191,7 +1238,7 @@
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="27"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
@@ -1218,7 +1265,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1228,7 +1275,7 @@
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
@@ -1236,7 +1283,7 @@
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
@@ -1244,7 +1291,7 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="28"/>
+      <c r="F33" s="39"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -1252,7 +1299,7 @@
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="28"/>
+      <c r="F34" s="39"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
@@ -1262,7 +1309,7 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="27"/>
+      <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
@@ -1400,10 +1447,10 @@
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="29"/>
+      <c r="B49" s="40"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="21"/>
@@ -1457,44 +1504,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1595,17 +1642,17 @@
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="30" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="37"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="29" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="16"/>
@@ -1673,7 +1720,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="34"/>
+      <c r="F26" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1689,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4A77FD-B06A-CC44-B563-AB7667450FE9}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1703,44 +1750,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1824,7 +1871,7 @@
       <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="32" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="10"/>
@@ -1857,37 +1904,37 @@
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="30" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="37"/>
+      <c r="F22" s="31"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="30" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="37"/>
+      <c r="F23" s="31"/>
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="30" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="37"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="33" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="16"/>
@@ -1940,7 +1987,7 @@
     </row>
     <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="30" t="s">
         <v>73</v>
       </c>
       <c r="C30" s="15"/>
@@ -1950,13 +1997,13 @@
     </row>
     <row r="31" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="29" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
-      <c r="F31" s="34"/>
+      <c r="F31" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1973,7 +2020,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1986,44 +2033,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2106,7 +2153,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="37" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2118,7 +2165,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -2128,7 +2175,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -2138,7 +2185,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -2148,27 +2195,27 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="37" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2180,7 +2227,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="26"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -2190,7 +2237,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -2200,7 +2247,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -2210,17 +2257,17 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="26"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41" t="s">
+      <c r="A28" s="34"/>
+      <c r="B28" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="27"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
@@ -2241,7 +2288,7 @@
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D31" s="10"/>
@@ -2258,7 +2305,7 @@
     </row>
     <row r="33" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="30" t="s">
         <v>87</v>
       </c>
       <c r="C33" s="15"/>
@@ -2268,13 +2315,13 @@
     </row>
     <row r="34" spans="1:6" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="29" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
-      <c r="F34" s="34"/>
+      <c r="F34" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2293,7 +2340,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2306,44 +2353,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2426,7 +2473,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="37" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2438,7 +2485,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -2448,7 +2495,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -2458,7 +2505,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -2468,21 +2515,21 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="30" t="s">
         <v>97</v>
       </c>
       <c r="C23" s="15"/>
@@ -2492,13 +2539,13 @@
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="26"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -2508,7 +2555,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
@@ -2518,7 +2565,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="27"/>
+      <c r="F26" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2530,4 +2577,328 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C17115-A3C4-344A-9F74-0F2EBB6B4AA7}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>68</v>
+      </c>
+      <c r="E16" s="5">
+        <v>55</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="37"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="37"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="44"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="26"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="37"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="37"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="37"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="37"/>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="37"/>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="37"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="37"/>
+    </row>
+    <row r="33" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="F24:F34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding initial web app
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB96AA3-F961-6747-8F1A-B2B452E4146D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40C78B-7019-8D49-889C-5F911AD2D7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="103800" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="103800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -447,6 +447,9 @@
 3 Changes: 3
 4+ Changes: 4
 </t>
+  </si>
+  <si>
+    <t>Infrastructure-specific</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984F1C9-37A0-284B-A0D6-38654FE3C443}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1208,7 @@
     <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="15" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
@@ -2020,7 +2023,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2160,7 +2163,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="15" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
@@ -2340,7 +2343,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2480,7 +2483,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="15" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
@@ -2583,8 +2586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C17115-A3C4-344A-9F74-0F2EBB6B4AA7}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,7 +2727,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="15" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>

</xml_diff>

<commit_message>
adding website, api, and processor
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40C78B-7019-8D49-889C-5F911AD2D7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12529F1-A5A0-F940-8B16-F4FF80ABA398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="103800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="103800" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>Infrastructure-specific</t>
+  </si>
+  <si>
+    <t>Successfully configured and demonstrated a Blue-Green deployment</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984F1C9-37A0-284B-A0D6-38654FE3C443}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2584,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C17115-A3C4-344A-9F74-0F2EBB6B4AA7}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2701,14 +2704,14 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5">
-        <f>SUM(C17:C34)</f>
+        <f>SUM(C17:C35)</f>
         <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E16" s="5">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F16" s="21"/>
     </row>
@@ -2807,7 +2810,7 @@
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="30" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
@@ -2817,7 +2820,7 @@
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
@@ -2827,7 +2830,7 @@
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="14"/>
@@ -2837,7 +2840,7 @@
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="14"/>
@@ -2847,7 +2850,7 @@
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="14"/>
@@ -2857,17 +2860,17 @@
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="30" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="37"/>
     </row>
-    <row r="32" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
-      <c r="B32" s="15" t="s">
-        <v>95</v>
+      <c r="B32" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="14"/>
@@ -2876,23 +2879,33 @@
     </row>
     <row r="33" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
-      <c r="B33" s="45" t="s">
-        <v>102</v>
+      <c r="B33" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="37"/>
     </row>
-    <row r="34" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16" t="s">
+    <row r="34" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="38"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2900,7 +2913,7 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="F17:F22"/>
-    <mergeCell ref="F24:F34"/>
+    <mergeCell ref="F24:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding success criteria for challenge 7 coaches guide
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DDEBD5-3E58-0840-B36B-4DC6D38D4E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3998CF-8E26-F145-A2D1-A5283D062E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="6" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Challenge 4" sheetId="4" r:id="rId4"/>
     <sheet name="Challenge 5" sheetId="5" r:id="rId5"/>
     <sheet name="Challenge 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Challenge 6 (2)" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="126">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -453,6 +454,42 @@
   </si>
   <si>
     <t>Successfully configured a hot-hot, multi-region deployment</t>
+  </si>
+  <si>
+    <t>Challenge 7: Optimizing the API</t>
+  </si>
+  <si>
+    <t>Deploying the API to Serverless</t>
+  </si>
+  <si>
+    <t>Refactored and deployed the Web API solution to Azure Functions</t>
+  </si>
+  <si>
+    <t>Azure Functions' App Service is separate from front end</t>
+  </si>
+  <si>
+    <t>Application Insights in enabled</t>
+  </si>
+  <si>
+    <t>Azure DevOps pipelines have been updated to build and deploy</t>
+  </si>
+  <si>
+    <t>Azure Functions instance deployed by Azure Bicep</t>
+  </si>
+  <si>
+    <t>Azure Functions configured to scale</t>
+  </si>
+  <si>
+    <t>Azure Key Vault is configured and connected for storing secrets</t>
+  </si>
+  <si>
+    <t>Grafana dashboards have been updated</t>
+  </si>
+  <si>
+    <t>Azure Functions have been securely placed behind APIM</t>
+  </si>
+  <si>
+    <t>CORS has been configured</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984F1C9-37A0-284B-A0D6-38654FE3C443}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2917,4 +2954,245 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18C34BA-BCFC-C343-B2D9-E45D0484D199}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5">
+        <v>32</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="38"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typo in successMatrix
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270BC7F2-4677-F74E-9F79-BB492E1CB653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1706300F-0FBA-A24A-9910-1300C72D18D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="6" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Challenge 4" sheetId="4" r:id="rId4"/>
     <sheet name="Challenge 5" sheetId="5" r:id="rId5"/>
     <sheet name="Challenge 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Challenge 6 (2)" sheetId="7" r:id="rId7"/>
+    <sheet name="Challenge 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2961,7 +2961,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updating successMatrix with Challenge 8 requirements
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1706300F-0FBA-A24A-9910-1300C72D18D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D83CA9D-62F2-5F48-8388-DC2F5AEFC635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="6" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="7" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Challenge 5" sheetId="5" r:id="rId5"/>
     <sheet name="Challenge 6" sheetId="6" r:id="rId6"/>
     <sheet name="Challenge 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Challenge 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="132">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -490,6 +491,24 @@
   </si>
   <si>
     <t>CORS has been configured</t>
+  </si>
+  <si>
+    <t>Challenge 8: Tightening database security</t>
+  </si>
+  <si>
+    <t>Applying security to the database</t>
+  </si>
+  <si>
+    <t>Successfully encrypted all columns in the [Accounts] table</t>
+  </si>
+  <si>
+    <t>Successfully encrypted the [Users] table</t>
+  </si>
+  <si>
+    <t>Successfully encrypted the [Tranactions].[AccountId] column</t>
+  </si>
+  <si>
+    <t>Application connectivity to the database is conducted via a managed principal</t>
   </si>
 </sst>
 </file>
@@ -633,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -723,6 +742,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2960,7 +2982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18C34BA-BCFC-C343-B2D9-E45D0484D199}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -3195,4 +3217,185 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C43AC4-C3F4-F942-A2B5-C15664C4B04E}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5">
+        <v>13</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding challenge 9 successmatrix
</commit_message>
<xml_diff>
--- a/guides/successMatrix.xlsx
+++ b/guides/successMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10926"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/projects/microsoft/waf-oh/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D83CA9D-62F2-5F48-8388-DC2F5AEFC635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED06C8F-EA75-E84C-9C9C-2D2D3688C6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="7" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
+    <workbookView xWindow="101560" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{762185B8-AFDB-4C43-A7B2-8A5E7A74701C}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Challenge 6" sheetId="6" r:id="rId6"/>
     <sheet name="Challenge 7" sheetId="7" r:id="rId7"/>
     <sheet name="Challenge 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Challenge 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="138">
   <si>
     <t>Success Matrix</t>
   </si>
@@ -509,6 +510,24 @@
   </si>
   <si>
     <t>Application connectivity to the database is conducted via a managed principal</t>
+  </si>
+  <si>
+    <t>Challenge 9: Capturing correlation data</t>
+  </si>
+  <si>
+    <t>Capturing correlation data</t>
+  </si>
+  <si>
+    <t>Discussed ways in which to identify all components and correlating the life-cycle events of a single request.</t>
+  </si>
+  <si>
+    <t>Discussed what necessary data should be captured for troubleshooting.</t>
+  </si>
+  <si>
+    <t>Discussed how/where the data will be stored and queried while taking into consideration account privacy and PII.</t>
+  </si>
+  <si>
+    <t>Discussed and approach to validating issues, capturing them in a backlog, and testing the success or failure of mitigation.</t>
   </si>
 </sst>
 </file>
@@ -719,6 +738,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -742,9 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1076,37 +1095,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1263,7 +1282,7 @@
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1275,7 +1294,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -1285,7 +1304,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="38"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -1295,7 +1314,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="38"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -1303,7 +1322,7 @@
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="39"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
@@ -1330,7 +1349,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="41" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1340,7 +1359,7 @@
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="40"/>
+      <c r="F31" s="41"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
@@ -1348,7 +1367,7 @@
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="40"/>
+      <c r="F32" s="41"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
@@ -1356,7 +1375,7 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="40"/>
+      <c r="F33" s="41"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -1364,7 +1383,7 @@
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="40"/>
+      <c r="F34" s="41"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
@@ -1374,7 +1393,7 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="39"/>
+      <c r="F35" s="40"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
@@ -1512,10 +1531,10 @@
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="41"/>
+      <c r="B49" s="42"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="21"/>
@@ -1569,37 +1588,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1815,37 +1834,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2098,37 +2117,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2218,7 +2237,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="39" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2230,7 +2249,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -2240,7 +2259,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -2250,7 +2269,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -2260,7 +2279,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="38"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
@@ -2270,7 +2289,7 @@
       <c r="C22" s="34"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
-      <c r="F22" s="45"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
@@ -2280,7 +2299,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="38" t="s">
+      <c r="F23" s="39" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2292,7 +2311,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="38"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -2302,7 +2321,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -2312,7 +2331,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="38"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -2322,7 +2341,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="38"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
@@ -2332,7 +2351,7 @@
       <c r="C28" s="34"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
-      <c r="F28" s="39"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
@@ -2418,37 +2437,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2538,7 +2557,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="39" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2550,7 +2569,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -2560,7 +2579,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -2570,7 +2589,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -2580,7 +2599,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="38"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
@@ -2590,7 +2609,7 @@
       <c r="C22" s="34"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
-      <c r="F22" s="45"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
@@ -2610,7 +2629,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="38"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -2620,7 +2639,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
@@ -2630,7 +2649,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="39"/>
+      <c r="F26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2662,37 +2681,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2782,7 +2801,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="39" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2794,7 +2813,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -2804,7 +2823,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -2814,7 +2833,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -2824,7 +2843,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="38"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
@@ -2834,7 +2853,7 @@
       <c r="C22" s="34"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
-      <c r="F22" s="45"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
@@ -2854,7 +2873,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="38"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -2864,7 +2883,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
@@ -2874,7 +2893,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="38"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
@@ -2884,7 +2903,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="38"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
@@ -2894,7 +2913,7 @@
       <c r="C28" s="15"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="38"/>
+      <c r="F28" s="39"/>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
@@ -2904,7 +2923,7 @@
       <c r="C29" s="15"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="38"/>
+      <c r="F29" s="39"/>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
@@ -2914,7 +2933,7 @@
       <c r="C30" s="15"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="38"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
@@ -2924,7 +2943,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="38"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
@@ -2934,7 +2953,7 @@
       <c r="C32" s="15"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
-      <c r="F32" s="38"/>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
@@ -2944,7 +2963,7 @@
       <c r="C33" s="15"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="38"/>
+      <c r="F33" s="39"/>
     </row>
     <row r="34" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
@@ -2954,7 +2973,7 @@
       <c r="C34" s="15"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
-      <c r="F34" s="38"/>
+      <c r="F34" s="39"/>
     </row>
     <row r="35" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
@@ -2964,7 +2983,7 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="39"/>
+      <c r="F35" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2996,37 +3015,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3116,7 +3135,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="38"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
@@ -3126,7 +3145,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -3136,7 +3155,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -3146,7 +3165,7 @@
       <c r="C20" s="15"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="38"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
@@ -3156,7 +3175,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="38"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
@@ -3166,7 +3185,7 @@
       <c r="C22" s="15"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="38"/>
+      <c r="F22" s="39"/>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
@@ -3176,7 +3195,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="38"/>
+      <c r="F23" s="39"/>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
@@ -3186,7 +3205,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="38"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
@@ -3196,7 +3215,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
@@ -3206,7 +3225,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="39"/>
+      <c r="F26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3223,7 +3242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C43AC4-C3F4-F942-A2B5-C15664C4B04E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3237,37 +3256,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3357,7 +3376,7 @@
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="38"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
@@ -3367,7 +3386,7 @@
       <c r="C18" s="15"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
@@ -3377,17 +3396,198 @@
       <c r="C19" s="15"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="38" t="s">
         <v>131</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="39"/>
+      <c r="F20" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="F17:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046E7E0D-01AC-8043-81A5-8FA6ABF9F53F}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <f>SUM(C17:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5">
+        <v>13</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>